<commit_message>
Implementierungsplan - Klassen integriert.
</commit_message>
<xml_diff>
--- a/2-Entwurf/2-Entwicklung/ImplementierungsPlan/Implementierungsplan.xlsx
+++ b/2-Entwurf/2-Entwicklung/ImplementierungsPlan/Implementierungsplan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF18E7C2-071A-49BA-ACD2-890CBD7183AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976F120D-A15F-4987-BF79-1E471AF058A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="115">
   <si>
     <t>Woche</t>
   </si>
@@ -38,6 +38,333 @@
   </si>
   <si>
     <t>GUI</t>
+  </si>
+  <si>
+    <t>Cache</t>
+  </si>
+  <si>
+    <t>MRunTiming</t>
+  </si>
+  <si>
+    <t>Timer</t>
+  </si>
+  <si>
+    <t>BufferForOneSensorInChannel</t>
+  </si>
+  <si>
+    <t>TimestampValuePair</t>
+  </si>
+  <si>
+    <t>ConnectionTerminatedAction</t>
+  </si>
+  <si>
+    <t>TimeoutAction</t>
+  </si>
+  <si>
+    <t>ErrorCodeAction</t>
+  </si>
+  <si>
+    <t>DataSetCompleteAction</t>
+  </si>
+  <si>
+    <t>EnhancedValuePacket</t>
+  </si>
+  <si>
+    <t>ErrorCodesForInChannel</t>
+  </si>
+  <si>
+    <t>CheckAndNotifyAction</t>
+  </si>
+  <si>
+    <t>IMRunListener</t>
+  </si>
+  <si>
+    <t>IMRunInfo</t>
+  </si>
+  <si>
+    <t>TimerTask</t>
+  </si>
+  <si>
+    <t>Controller</t>
+  </si>
+  <si>
+    <t>Submodul</t>
+  </si>
+  <si>
+    <t>Model Interface</t>
+  </si>
+  <si>
+    <t>IModelInformation</t>
+  </si>
+  <si>
+    <t>IMeasurementRun</t>
+  </si>
+  <si>
+    <t>View Controller Interface</t>
+  </si>
+  <si>
+    <t>ButtonAction</t>
+  </si>
+  <si>
+    <t>BlockAction</t>
+  </si>
+  <si>
+    <t>ConnectionAction</t>
+  </si>
+  <si>
+    <t>Command Pattern</t>
+  </si>
+  <si>
+    <t>CommandManager</t>
+  </si>
+  <si>
+    <t>Command</t>
+  </si>
+  <si>
+    <t>AddBlockToConfigCommand</t>
+  </si>
+  <si>
+    <t>ModifyBlockInConfigCommand</t>
+  </si>
+  <si>
+    <t>RemoveBlockFromConfigCommand</t>
+  </si>
+  <si>
+    <t>EditBlockPropertiesCommand</t>
+  </si>
+  <si>
+    <t>CloneBlockCommand</t>
+  </si>
+  <si>
+    <t>ExportBlockPrototypeCommand</t>
+  </si>
+  <si>
+    <t>SaveConfigCommand</t>
+  </si>
+  <si>
+    <t>LoadConfigCommand</t>
+  </si>
+  <si>
+    <t>ResetConfigCommand</t>
+  </si>
+  <si>
+    <t>CreateChannelConnectionCommand</t>
+  </si>
+  <si>
+    <t>ModifyChannelConnectionCommand</t>
+  </si>
+  <si>
+    <t>DeleteChannelConnectionCommand</t>
+  </si>
+  <si>
+    <t>StartRunCommand</t>
+  </si>
+  <si>
+    <t>StopRunCommand</t>
+  </si>
+  <si>
+    <t>ResumeRunCommand</t>
+  </si>
+  <si>
+    <t>FileService</t>
+  </si>
+  <si>
+    <t>CsvService</t>
+  </si>
+  <si>
+    <t>PngService</t>
+  </si>
+  <si>
+    <t>YamlService</t>
+  </si>
+  <si>
+    <t>MainWindow</t>
+  </si>
+  <si>
+    <t>Menues</t>
+  </si>
+  <si>
+    <t>PrototypeField</t>
+  </si>
+  <si>
+    <t>TransformationBlockField</t>
+  </si>
+  <si>
+    <t>RepresentationBlockField</t>
+  </si>
+  <si>
+    <t>FieldHandler</t>
+  </si>
+  <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t>ConfigurationField</t>
+  </si>
+  <si>
+    <t>BlockDragAndDropHandler</t>
+  </si>
+  <si>
+    <t>BuildingBlockView</t>
+  </si>
+  <si>
+    <t>SensorBlockView</t>
+  </si>
+  <si>
+    <t>TransformationBlockView</t>
+  </si>
+  <si>
+    <t>RepresentationBlockView</t>
+  </si>
+  <si>
+    <t>HelpDecoratorHandler</t>
+  </si>
+  <si>
+    <t>AddWireDragAndDropHandler</t>
+  </si>
+  <si>
+    <t>RemoveWireDragAndDropHandler</t>
+  </si>
+  <si>
+    <t>ChannelDecorator</t>
+  </si>
+  <si>
+    <t>OutChannelDecorator</t>
+  </si>
+  <si>
+    <t>InChannelDecorator</t>
+  </si>
+  <si>
+    <t>Wire</t>
+  </si>
+  <si>
+    <t>BuildingBlockProperties</t>
+  </si>
+  <si>
+    <t>BuildingBlockPropertiesHandler</t>
+  </si>
+  <si>
+    <t>SensorBlockProperties</t>
+  </si>
+  <si>
+    <t>TransformationBlockProperties</t>
+  </si>
+  <si>
+    <t>TransBlockPropertiesHandler</t>
+  </si>
+  <si>
+    <t>RepresentationBlockProperties</t>
+  </si>
+  <si>
+    <t>ReprBlockPropertiesHandler</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>ButtonHandler</t>
+  </si>
+  <si>
+    <t>Exception</t>
+  </si>
+  <si>
+    <t>ExceptionWindowManager</t>
+  </si>
+  <si>
+    <t>ExceptionWindow</t>
+  </si>
+  <si>
+    <t>BuildingBlockExceptionWindow</t>
+  </si>
+  <si>
+    <t>ConnectionExceptionWindow</t>
+  </si>
+  <si>
+    <t>GeneralExceptionWindow</t>
+  </si>
+  <si>
+    <t>HelpAndOption</t>
+  </si>
+  <si>
+    <t>OptionsWindow</t>
+  </si>
+  <si>
+    <t>HelpWindow</t>
+  </si>
+  <si>
+    <t>HelpWindowHandler</t>
+  </si>
+  <si>
+    <t>OptionsWindowHandler</t>
+  </si>
+  <si>
+    <t>FacadeControllerView</t>
+  </si>
+  <si>
+    <t>PickUpPointControllerView</t>
+  </si>
+  <si>
+    <t>IButtonAction</t>
+  </si>
+  <si>
+    <t>IBlockAction</t>
+  </si>
+  <si>
+    <t>IConnectionAction</t>
+  </si>
+  <si>
+    <t>FacadeModelView</t>
+  </si>
+  <si>
+    <t>ViewDirectoryInterface</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Core</t>
+  </si>
+  <si>
+    <t>MeasurementRun</t>
+  </si>
+  <si>
+    <t>MesurementRunState</t>
+  </si>
+  <si>
+    <t>MeasurementConfiguration</t>
+  </si>
+  <si>
+    <t>BuildingBlock</t>
+  </si>
+  <si>
+    <t>HelpMessage</t>
+  </si>
+  <si>
+    <t>YamlRepresentation</t>
+  </si>
+  <si>
+    <t>BuildingBlockDirectory</t>
+  </si>
+  <si>
+    <t>TransformationLogic</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>RepresentationLogic</t>
+  </si>
+  <si>
+    <t>Transformation</t>
+  </si>
+  <si>
+    <t>Representation</t>
+  </si>
+  <si>
+    <t>TableRespresentation</t>
+  </si>
+  <si>
+    <t>XYRepresentation</t>
   </si>
 </sst>
 </file>
@@ -87,17 +414,25 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -373,192 +708,194 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BP8"/>
+  <dimension ref="A1:BQ120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="25.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="12" width="10.28515625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="18.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="25.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="7" max="13" width="10.28515625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="D1" s="1" t="s">
+    <row r="1" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
+    <row r="2" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>27</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="4">
         <v>28</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3">
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4">
         <v>29</v>
       </c>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3">
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4">
         <v>30</v>
       </c>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3">
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4">
         <v>31</v>
       </c>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="3"/>
-      <c r="AG2" s="3"/>
-      <c r="AH2" s="3">
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4"/>
+      <c r="AF2" s="4"/>
+      <c r="AG2" s="4"/>
+      <c r="AH2" s="4"/>
+      <c r="AI2" s="4">
         <v>32</v>
       </c>
-      <c r="AI2" s="3"/>
-      <c r="AJ2" s="3"/>
-      <c r="AK2" s="3"/>
-      <c r="AL2" s="3"/>
-      <c r="AM2" s="3"/>
-      <c r="AN2" s="3"/>
-    </row>
-    <row r="3" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="C3" s="1" t="s">
+      <c r="AJ2" s="4"/>
+      <c r="AK2" s="4"/>
+      <c r="AL2" s="4"/>
+      <c r="AM2" s="4"/>
+      <c r="AN2" s="4"/>
+      <c r="AO2" s="4"/>
+    </row>
+    <row r="3" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>43653</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>43654</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>43655</v>
       </c>
-      <c r="H3" s="2">
+      <c r="I3" s="2">
         <v>43656</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <v>43657</v>
       </c>
-      <c r="J3" s="2">
+      <c r="K3" s="2">
         <v>43658</v>
       </c>
-      <c r="K3" s="2">
+      <c r="L3" s="2">
         <v>43659</v>
       </c>
-      <c r="L3" s="2">
+      <c r="M3" s="2">
         <v>43660</v>
       </c>
-      <c r="M3" s="2">
+      <c r="N3" s="2">
         <v>43661</v>
       </c>
-      <c r="N3" s="2">
+      <c r="O3" s="2">
         <v>43662</v>
       </c>
-      <c r="O3" s="2">
+      <c r="P3" s="2">
         <v>43663</v>
       </c>
-      <c r="P3" s="2">
+      <c r="Q3" s="2">
         <v>43664</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="R3" s="2">
         <v>43665</v>
       </c>
-      <c r="R3" s="2">
+      <c r="S3" s="2">
         <v>43666</v>
       </c>
-      <c r="S3" s="2">
+      <c r="T3" s="2">
         <v>43667</v>
       </c>
-      <c r="T3" s="2">
+      <c r="U3" s="2">
         <v>43668</v>
       </c>
-      <c r="U3" s="2">
+      <c r="V3" s="2">
         <v>43669</v>
       </c>
-      <c r="V3" s="2">
+      <c r="W3" s="2">
         <v>43670</v>
       </c>
-      <c r="W3" s="2">
+      <c r="X3" s="2">
         <v>43671</v>
       </c>
-      <c r="X3" s="2">
+      <c r="Y3" s="2">
         <v>43672</v>
       </c>
-      <c r="Y3" s="2">
+      <c r="Z3" s="2">
         <v>43673</v>
       </c>
-      <c r="Z3" s="2">
+      <c r="AA3" s="2">
         <v>43674</v>
       </c>
-      <c r="AA3" s="2">
+      <c r="AB3" s="2">
         <v>43675</v>
       </c>
-      <c r="AB3" s="2">
+      <c r="AC3" s="2">
         <v>43676</v>
       </c>
-      <c r="AC3" s="2">
+      <c r="AD3" s="2">
         <v>43677</v>
       </c>
-      <c r="AD3" s="2">
+      <c r="AE3" s="2">
         <v>43678</v>
       </c>
-      <c r="AE3" s="2">
+      <c r="AF3" s="2">
         <v>43679</v>
       </c>
-      <c r="AF3" s="2">
+      <c r="AG3" s="2">
         <v>43680</v>
       </c>
-      <c r="AG3" s="2">
+      <c r="AH3" s="2">
         <v>43681</v>
       </c>
-      <c r="AH3" s="2">
+      <c r="AI3" s="2">
         <v>43682</v>
       </c>
-      <c r="AI3" s="2">
+      <c r="AJ3" s="2">
         <v>43683</v>
       </c>
-      <c r="AJ3" s="2">
+      <c r="AK3" s="2">
         <v>43684</v>
       </c>
-      <c r="AK3" s="2">
+      <c r="AL3" s="2">
         <v>43685</v>
       </c>
-      <c r="AL3" s="2">
+      <c r="AM3" s="2">
         <v>43686</v>
       </c>
-      <c r="AM3" s="2">
+      <c r="AN3" s="2">
         <v>43687</v>
       </c>
-      <c r="AN3" s="2">
+      <c r="AO3" s="2">
         <v>43688</v>
       </c>
-      <c r="AO3" s="2"/>
       <c r="AP3" s="2"/>
       <c r="AQ3" s="2"/>
       <c r="AR3" s="2"/>
@@ -586,32 +923,594 @@
       <c r="BN3" s="2"/>
       <c r="BO3" s="2"/>
       <c r="BP3" s="2"/>
-    </row>
-    <row r="4" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="BQ3" s="2"/>
+    </row>
+    <row r="4" spans="1:69" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:69" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:69" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C39" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C40" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C41" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C42" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C43" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C44" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C45" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C46" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C47" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C48" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C49" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C50" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C52" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C53" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C54" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C56" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C58" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C59" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C60" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C61" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B62" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C63" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C64" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C65" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C66" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C67" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C68" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C69" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C70" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C71" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C72" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C73" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C74" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C75" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B76" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C77" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C78" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C79" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C80" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C81" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C82" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C83" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B84" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C85" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C86" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B87" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C88" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C89" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C90" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C91" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C92" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B93" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C94" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C95" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C96" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C97" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B98" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C99" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C100" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C101" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C102" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B103" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C104" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B106" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C107" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C108" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C109" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C110" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C111" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C112" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C113" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B114" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C115" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C116" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B117" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C118" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C119" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C120" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="F2:L2"/>
-    <mergeCell ref="M2:S2"/>
-    <mergeCell ref="T2:Z2"/>
-    <mergeCell ref="AA2:AG2"/>
-    <mergeCell ref="AH2:AN2"/>
+    <mergeCell ref="G2:M2"/>
+    <mergeCell ref="N2:T2"/>
+    <mergeCell ref="U2:AA2"/>
+    <mergeCell ref="AB2:AH2"/>
+    <mergeCell ref="AI2:AO2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>